<commit_message>
Added char concept and planning update
</commit_message>
<xml_diff>
--- a/Documentation/Asset list & planning.xlsx
+++ b/Documentation/Asset list & planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="233">
   <si>
     <t>Probation Area</t>
   </si>
@@ -657,6 +657,72 @@
   </si>
   <si>
     <t>Lara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characters </t>
+  </si>
+  <si>
+    <t>Dokter</t>
+  </si>
+  <si>
+    <t>Assistant 1</t>
+  </si>
+  <si>
+    <t>Assistant 2</t>
+  </si>
+  <si>
+    <t>Client 1</t>
+  </si>
+  <si>
+    <t>Client 2</t>
+  </si>
+  <si>
+    <t>Client 3</t>
+  </si>
+  <si>
+    <t>Client 4</t>
+  </si>
+  <si>
+    <t>Client 5</t>
+  </si>
+  <si>
+    <t>Client 6</t>
+  </si>
+  <si>
+    <t>Client 7</t>
+  </si>
+  <si>
+    <t>3D_CHAR_Dokter</t>
+  </si>
+  <si>
+    <t>3D_CHAR_Assistant1</t>
+  </si>
+  <si>
+    <t>3D_CHAR_Client1</t>
+  </si>
+  <si>
+    <t>3D_CHAR_Assistant2</t>
+  </si>
+  <si>
+    <t>3D_CHAR_Client2</t>
+  </si>
+  <si>
+    <t>3D_CHAR_Client3</t>
+  </si>
+  <si>
+    <t>3D_CHAR_Client4</t>
+  </si>
+  <si>
+    <t>3D_CHAR_Client5</t>
+  </si>
+  <si>
+    <t>3D_CHAR_Client6</t>
+  </si>
+  <si>
+    <t>3D_CHAR_Client7</t>
+  </si>
+  <si>
+    <t>Hadewij</t>
   </si>
 </sst>
 </file>
@@ -1206,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S141"/>
+  <dimension ref="A1:S153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,7 +1337,9 @@
       <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1318,14 +1386,18 @@
       <c r="D5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1352,7 +1424,9 @@
       <c r="I6" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>207</v>
+      </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1408,7 +1482,9 @@
       <c r="I8" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1462,7 +1538,9 @@
       <c r="I10" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="J10" s="2"/>
+      <c r="J10" s="9" t="s">
+        <v>207</v>
+      </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -3857,6 +3935,145 @@
       <c r="E141" s="17"/>
       <c r="F141" s="18"/>
     </row>
+    <row r="142" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F143" s="2"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" s="23"/>
+      <c r="B144" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D144" s="2"/>
+      <c r="E144" s="5"/>
+      <c r="F144" s="2"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="23"/>
+      <c r="B145" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D145" s="2"/>
+      <c r="E145" s="5"/>
+      <c r="F145" s="2"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="23"/>
+      <c r="B146" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D146" s="2"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="2"/>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="23"/>
+      <c r="B147" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C147" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D147" s="2"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="2"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="23"/>
+      <c r="B148" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C148" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D148" s="2"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="2"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="23"/>
+      <c r="B149" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D149" s="2"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="2"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="23"/>
+      <c r="B150" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C150" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D150" s="2"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="2"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="23"/>
+      <c r="B151" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C151" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D151" s="2"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="2"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="23"/>
+      <c r="B152" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D152" s="2"/>
+      <c r="E152" s="5"/>
+      <c r="F152" s="2"/>
+    </row>
+    <row r="153" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="24"/>
+      <c r="B153" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C153" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="D153" s="7"/>
+      <c r="E153" s="8"/>
+      <c r="F153" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Planning push voor marc
</commit_message>
<xml_diff>
--- a/Documentation/Asset list & planning.xlsx
+++ b/Documentation/Asset list & planning.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="282">
   <si>
     <t>Probation Area</t>
   </si>
@@ -723,13 +724,160 @@
   </si>
   <si>
     <t>Hadewij</t>
+  </si>
+  <si>
+    <t>Rack</t>
+  </si>
+  <si>
+    <t>Glass display</t>
+  </si>
+  <si>
+    <t>Trashcan</t>
+  </si>
+  <si>
+    <t>3D_ENV_GEN_Rack</t>
+  </si>
+  <si>
+    <t>3D_ENV_GEN_Glass display</t>
+  </si>
+  <si>
+    <t>Transporter bed</t>
+  </si>
+  <si>
+    <t>Transporter rails straight</t>
+  </si>
+  <si>
+    <t>Transporter rails curve</t>
+  </si>
+  <si>
+    <t>Hairdryer</t>
+  </si>
+  <si>
+    <t>Sodium bottle</t>
+  </si>
+  <si>
+    <t>Shower tile</t>
+  </si>
+  <si>
+    <t>Shower</t>
+  </si>
+  <si>
+    <t>Hatch</t>
+  </si>
+  <si>
+    <t>Morgue door</t>
+  </si>
+  <si>
+    <t>Transporter control panel</t>
+  </si>
+  <si>
+    <t>Power supply puzzle</t>
+  </si>
+  <si>
+    <t>Examination bed</t>
+  </si>
+  <si>
+    <t>Robot arms</t>
+  </si>
+  <si>
+    <t>Surgery Equipement</t>
+  </si>
+  <si>
+    <t>Brains on sticks</t>
+  </si>
+  <si>
+    <t>Locker doors</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_TransporterBed</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_TransporterRailsStriaght</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_ShowerTile</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_MorgueDoor</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_ExaminationBed</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_RobotArms</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_TransporterRailsCurve</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_Hairdryer</t>
+  </si>
+  <si>
+    <t>3D_ENV_ITEM_SodiumBottle</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_Shower</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_Hatch</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_DoorDisplay</t>
+  </si>
+  <si>
+    <t>Door display</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_TransporterControlPanel</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_PowerSupplyPuzzle</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_SurgeryEquipments</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_BrainsOnSticks</t>
+  </si>
+  <si>
+    <t>3D_ENV_MORG_LockerDoors</t>
+  </si>
+  <si>
+    <t>Assetlist</t>
+  </si>
+  <si>
+    <t>Particles</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodium </t>
+  </si>
+  <si>
+    <t>Lazer</t>
+  </si>
+  <si>
+    <t>3D_PART_Fire</t>
+  </si>
+  <si>
+    <t>3D_PART_Shower</t>
+  </si>
+  <si>
+    <t>3D_PART_Sodium</t>
+  </si>
+  <si>
+    <t>3D_PART_Lazer</t>
+  </si>
+  <si>
+    <t>Planning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,6 +890,13 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -924,7 +1079,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -958,6 +1113,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1272,24 +1433,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S153"/>
+  <dimension ref="A1:S179"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.140625" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>272</v>
+      </c>
+    </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>0</v>
@@ -1651,7 +1816,9 @@
       <c r="F14" s="5"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="I14" s="9" t="s">
+        <v>233</v>
+      </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1678,7 +1845,9 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="I15" s="9" t="s">
+        <v>234</v>
+      </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -3570,53 +3739,71 @@
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="14"/>
       <c r="B106" s="1"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="2"/>
+      <c r="C106" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="E106" s="9"/>
       <c r="F106" s="5"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="14"/>
       <c r="B107" s="1"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
+      <c r="C107" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="E107" s="9"/>
       <c r="F107" s="5"/>
     </row>
-    <row r="108" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="14"/>
-      <c r="B108" s="6"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="7"/>
-      <c r="E108" s="7"/>
-      <c r="F108" s="8"/>
-    </row>
-    <row r="109" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="1"/>
+      <c r="C108" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="14"/>
-      <c r="B109" s="6"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="7"/>
-      <c r="E109" s="7"/>
-      <c r="F109" s="8"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="14"/>
-      <c r="B110" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="4"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="E110" s="2"/>
+      <c r="F110" s="5"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="14"/>
       <c r="B111" s="1"/>
-      <c r="C111" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>194</v>
+      <c r="C111" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>255</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111" s="5"/>
@@ -3624,458 +3811,752 @@
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="14"/>
       <c r="B112" s="1"/>
-      <c r="C112" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D112" s="2"/>
-      <c r="E112" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C112" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D112" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E112" s="2"/>
+      <c r="F112" s="5"/>
+    </row>
+    <row r="113" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="14"/>
       <c r="B113" s="1"/>
-      <c r="C113" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D113" s="2"/>
+      <c r="C113" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="D113" s="33" t="s">
+        <v>261</v>
+      </c>
       <c r="E113" s="2"/>
-      <c r="F113" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F113" s="5"/>
+    </row>
+    <row r="114" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
       <c r="B114" s="1"/>
-      <c r="C114" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>209</v>
+      <c r="C114" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D114" s="33" t="s">
+        <v>262</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" s="5"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="14"/>
       <c r="B115" s="1"/>
       <c r="C115" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>96</v>
+        <v>243</v>
+      </c>
+      <c r="D115" s="33" t="s">
+        <v>256</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115" s="5"/>
     </row>
-    <row r="116" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="14"/>
       <c r="B116" s="1"/>
       <c r="C116" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>97</v>
+        <v>244</v>
+      </c>
+      <c r="D116" s="33" t="s">
+        <v>263</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116" s="5"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="14"/>
-      <c r="B117" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="4"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B117" s="1"/>
+      <c r="C117" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D117" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="E117" s="2"/>
+      <c r="F117" s="5"/>
+    </row>
+    <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="14"/>
       <c r="B118" s="1"/>
       <c r="C118" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D118" s="9" t="s">
-        <v>198</v>
+        <v>266</v>
+      </c>
+      <c r="D118" s="33" t="s">
+        <v>265</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118" s="5"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
       <c r="B119" s="1"/>
       <c r="C119" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D119" s="9" t="s">
-        <v>196</v>
+        <v>246</v>
+      </c>
+      <c r="D119" s="33" t="s">
+        <v>257</v>
       </c>
       <c r="E119" s="2"/>
       <c r="F119" s="5"/>
     </row>
-    <row r="120" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="15"/>
-      <c r="B120" s="6"/>
-      <c r="C120" s="7"/>
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
-      <c r="F120" s="8"/>
-    </row>
-    <row r="121" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="9"/>
-      <c r="B121" s="9"/>
-      <c r="C121" s="9"/>
-      <c r="D121" s="9"/>
-      <c r="E121" s="9"/>
-      <c r="F121" s="9"/>
-    </row>
-    <row r="122" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E122" s="3"/>
-      <c r="F122" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="14"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D120" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="E120" s="2"/>
+      <c r="F120" s="5"/>
+    </row>
+    <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="14"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D121" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="5"/>
+    </row>
+    <row r="122" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="14"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="D122" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="E122" s="2"/>
+      <c r="F122" s="5"/>
+    </row>
+    <row r="123" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
-      <c r="B123" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3"/>
-      <c r="F123" s="4"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B123" s="1"/>
+      <c r="C123" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D123" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="E123" s="2"/>
+      <c r="F123" s="5"/>
+    </row>
+    <row r="124" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="14"/>
       <c r="B124" s="1"/>
-      <c r="C124" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>200</v>
+      <c r="C124" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D124" s="33" t="s">
+        <v>269</v>
       </c>
       <c r="E124" s="2"/>
       <c r="F124" s="5"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="14"/>
       <c r="B125" s="1"/>
-      <c r="C125" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>147</v>
+      <c r="C125" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D125" s="35" t="s">
+        <v>270</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125" s="5"/>
     </row>
-    <row r="126" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="14"/>
-      <c r="B126" s="6"/>
-      <c r="C126" s="7"/>
-      <c r="D126" s="7"/>
-      <c r="E126" s="7"/>
-      <c r="F126" s="8"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B126" s="1"/>
+      <c r="C126" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="D126" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="E126" s="2"/>
+      <c r="F126" s="5"/>
+    </row>
+    <row r="127" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="14"/>
-      <c r="B127" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
-      <c r="E127" s="3"/>
-      <c r="F127" s="4"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="7"/>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="8"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="14"/>
-      <c r="B128" s="1"/>
-      <c r="C128" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E128" s="2"/>
-      <c r="F128" s="5"/>
-    </row>
-    <row r="129" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B128" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="4"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="14"/>
-      <c r="B129" s="6"/>
-      <c r="C129" s="7"/>
-      <c r="D129" s="7"/>
-      <c r="E129" s="7"/>
-      <c r="F129" s="8"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E129" s="2"/>
+      <c r="F129" s="5"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="14"/>
-      <c r="B130" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
-      <c r="E130" s="3"/>
-      <c r="F130" s="4"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D130" s="2"/>
+      <c r="E130" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="14"/>
       <c r="B131" s="1"/>
       <c r="C131" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D131" s="2"/>
+      <c r="E131" s="2"/>
+      <c r="F131" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="14"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E132" s="2"/>
+      <c r="F132" s="5"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="14"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E133" s="2"/>
+      <c r="F133" s="5"/>
+    </row>
+    <row r="134" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="14"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E134" s="2"/>
+      <c r="F134" s="5"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="14"/>
+      <c r="B135" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="4"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="14"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D136" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E136" s="2"/>
+      <c r="F136" s="5"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="14"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D137" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E137" s="2"/>
+      <c r="F137" s="5"/>
+    </row>
+    <row r="138" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="15"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="7"/>
+      <c r="D138" s="7"/>
+      <c r="E138" s="7"/>
+      <c r="F138" s="8"/>
+    </row>
+    <row r="139" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="9"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+    </row>
+    <row r="140" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E140" s="3"/>
+      <c r="F140" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="14"/>
+      <c r="B141" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="4"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="14"/>
+      <c r="B142" s="1"/>
+      <c r="C142" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E142" s="2"/>
+      <c r="F142" s="5"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="14"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E143" s="2"/>
+      <c r="F143" s="5"/>
+    </row>
+    <row r="144" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="14"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="7"/>
+      <c r="D144" s="7"/>
+      <c r="E144" s="7"/>
+      <c r="F144" s="8"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" s="14"/>
+      <c r="B145" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
+      <c r="E145" s="3"/>
+      <c r="F145" s="4"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" s="14"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E146" s="2"/>
+      <c r="F146" s="5"/>
+    </row>
+    <row r="147" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="14"/>
+      <c r="B147" s="6"/>
+      <c r="C147" s="7"/>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
+      <c r="F147" s="8"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="14"/>
+      <c r="B148" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="4"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="14"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D131" s="2" t="s">
+      <c r="D149" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E131" s="2"/>
-      <c r="F131" s="5"/>
-    </row>
-    <row r="132" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="14"/>
-      <c r="B132" s="6"/>
-      <c r="C132" s="7"/>
-      <c r="D132" s="7"/>
-      <c r="E132" s="7"/>
-      <c r="F132" s="8"/>
-    </row>
-    <row r="133" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="22"/>
-      <c r="B133" s="25" t="s">
+      <c r="E149" s="2"/>
+      <c r="F149" s="5"/>
+    </row>
+    <row r="150" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="14"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="7"/>
+      <c r="D150" s="7"/>
+      <c r="E150" s="7"/>
+      <c r="F150" s="8"/>
+    </row>
+    <row r="151" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="22"/>
+      <c r="B151" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C133" s="3"/>
-      <c r="D133" s="3"/>
-      <c r="E133" s="3"/>
-      <c r="F133" s="4"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="20"/>
-      <c r="B134" s="30"/>
-      <c r="C134" s="9" t="s">
+      <c r="C151" s="3"/>
+      <c r="D151" s="3"/>
+      <c r="E151" s="3"/>
+      <c r="F151" s="4"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="20"/>
+      <c r="B152" s="30"/>
+      <c r="C152" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="D134" s="9" t="s">
+      <c r="D152" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="E134" s="9"/>
-      <c r="F134" s="26"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="20"/>
-      <c r="B135" s="23"/>
-      <c r="C135" s="9"/>
-      <c r="D135" s="9"/>
-      <c r="E135" s="9"/>
-      <c r="F135" s="26"/>
-    </row>
-    <row r="136" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="21"/>
-      <c r="B136" s="24"/>
-      <c r="C136" s="17"/>
-      <c r="D136" s="17"/>
-      <c r="E136" s="17"/>
-      <c r="F136" s="18"/>
-    </row>
-    <row r="137" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="9"/>
-      <c r="B137" s="9"/>
-      <c r="C137" s="9"/>
-      <c r="D137" s="9"/>
-      <c r="E137" s="9"/>
-      <c r="F137" s="9"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="31"/>
-      <c r="B138" s="31" t="s">
+      <c r="E152" s="9"/>
+      <c r="F152" s="26"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="20"/>
+      <c r="B153" s="23"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="26"/>
+    </row>
+    <row r="154" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="21"/>
+      <c r="B154" s="24"/>
+      <c r="C154" s="17"/>
+      <c r="D154" s="17"/>
+      <c r="E154" s="17"/>
+      <c r="F154" s="18"/>
+    </row>
+    <row r="155" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="9"/>
+      <c r="D155" s="9"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C138" s="28"/>
-      <c r="D138" s="28"/>
-      <c r="E138" s="28"/>
-      <c r="F138" s="29"/>
-    </row>
-    <row r="139" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A139" s="20"/>
-      <c r="B139" s="32"/>
-      <c r="C139" s="9" t="s">
+      <c r="B156" s="28"/>
+      <c r="C156" s="28"/>
+      <c r="D156" s="28"/>
+      <c r="E156" s="29"/>
+    </row>
+    <row r="157" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A157" s="32"/>
+      <c r="B157" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D139" s="9" t="s">
+      <c r="C157" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="E139" s="9"/>
-      <c r="F139" s="26"/>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="20"/>
-      <c r="B140" s="23"/>
-      <c r="C140" s="9"/>
-      <c r="D140" s="9"/>
-      <c r="E140" s="9"/>
-      <c r="F140" s="26"/>
-    </row>
-    <row r="141" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="21"/>
-      <c r="B141" s="24"/>
-      <c r="C141" s="17"/>
-      <c r="D141" s="17"/>
-      <c r="E141" s="17"/>
-      <c r="F141" s="18"/>
-    </row>
-    <row r="142" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="25" t="s">
+      <c r="D157" s="9"/>
+      <c r="E157" s="26"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="23"/>
+      <c r="B158" s="9"/>
+      <c r="C158" s="9"/>
+      <c r="D158" s="9"/>
+      <c r="E158" s="26"/>
+    </row>
+    <row r="159" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="24"/>
+      <c r="B159" s="17"/>
+      <c r="C159" s="17"/>
+      <c r="D159" s="17"/>
+      <c r="E159" s="18"/>
+    </row>
+    <row r="160" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="B143" s="3" t="s">
+      <c r="B161" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C143" s="3" t="s">
+      <c r="C161" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D143" s="3" t="s">
+      <c r="D161" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E143" s="4" t="s">
+      <c r="E161" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F143" s="2"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="23"/>
-      <c r="B144" s="2" t="s">
+      <c r="F161" s="2"/>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" s="23"/>
+      <c r="B162" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C144" s="2" t="s">
+      <c r="C162" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D144" s="2"/>
-      <c r="E144" s="5"/>
-      <c r="F144" s="2"/>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="23"/>
-      <c r="B145" s="2" t="s">
+      <c r="D162" s="2"/>
+      <c r="E162" s="5"/>
+      <c r="F162" s="2"/>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" s="23"/>
+      <c r="B163" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="C163" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D145" s="2"/>
-      <c r="E145" s="5"/>
-      <c r="F145" s="2"/>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="23"/>
-      <c r="B146" s="2" t="s">
+      <c r="D163" s="2"/>
+      <c r="E163" s="5"/>
+      <c r="F163" s="2"/>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="23"/>
+      <c r="B164" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C146" s="9" t="s">
+      <c r="C164" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D146" s="2"/>
-      <c r="E146" s="5"/>
-      <c r="F146" s="2"/>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="23"/>
-      <c r="B147" s="2" t="s">
+      <c r="D164" s="2"/>
+      <c r="E164" s="5"/>
+      <c r="F164" s="2"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" s="23"/>
+      <c r="B165" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C147" s="9" t="s">
+      <c r="C165" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="D147" s="2"/>
-      <c r="E147" s="5"/>
-      <c r="F147" s="2"/>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="23"/>
-      <c r="B148" s="2" t="s">
+      <c r="D165" s="2"/>
+      <c r="E165" s="5"/>
+      <c r="F165" s="2"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" s="23"/>
+      <c r="B166" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C148" s="9" t="s">
+      <c r="C166" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="D148" s="2"/>
-      <c r="E148" s="5"/>
-      <c r="F148" s="2"/>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="23"/>
-      <c r="B149" s="2" t="s">
+      <c r="D166" s="2"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="2"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" s="23"/>
+      <c r="B167" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C149" s="9" t="s">
+      <c r="C167" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="D149" s="2"/>
-      <c r="E149" s="5"/>
-      <c r="F149" s="2"/>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="23"/>
-      <c r="B150" s="2" t="s">
+      <c r="D167" s="2"/>
+      <c r="E167" s="5"/>
+      <c r="F167" s="2"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" s="23"/>
+      <c r="B168" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C150" s="9" t="s">
+      <c r="C168" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="D150" s="2"/>
-      <c r="E150" s="5"/>
-      <c r="F150" s="2"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="23"/>
-      <c r="B151" s="2" t="s">
+      <c r="D168" s="2"/>
+      <c r="E168" s="5"/>
+      <c r="F168" s="2"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" s="23"/>
+      <c r="B169" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C151" s="9" t="s">
+      <c r="C169" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="D151" s="2"/>
-      <c r="E151" s="5"/>
-      <c r="F151" s="2"/>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="23"/>
-      <c r="B152" s="2" t="s">
+      <c r="D169" s="2"/>
+      <c r="E169" s="5"/>
+      <c r="F169" s="2"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" s="23"/>
+      <c r="B170" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C152" s="9" t="s">
+      <c r="C170" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="D152" s="2"/>
-      <c r="E152" s="5"/>
-      <c r="F152" s="2"/>
-    </row>
-    <row r="153" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="24"/>
-      <c r="B153" s="7" t="s">
+      <c r="D170" s="2"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="2"/>
+    </row>
+    <row r="171" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="24"/>
+      <c r="B171" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="C153" s="17" t="s">
+      <c r="C171" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="D153" s="7"/>
-      <c r="E153" s="8"/>
-      <c r="F153" s="2"/>
+      <c r="D171" s="7"/>
+      <c r="E171" s="8"/>
+      <c r="F171" s="2"/>
+    </row>
+    <row r="172" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="B173" s="3"/>
+      <c r="C173" s="3"/>
+      <c r="D173" s="3"/>
+      <c r="E173" s="4"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" s="23"/>
+      <c r="B174" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C174" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D174" s="2"/>
+      <c r="E174" s="5"/>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" s="23"/>
+      <c r="B175" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C175" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="D175" s="2"/>
+      <c r="E175" s="5"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" s="23"/>
+      <c r="B176" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C176" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D176" s="2"/>
+      <c r="E176" s="5"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="23"/>
+      <c r="B177" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C177" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D177" s="2"/>
+      <c r="E177" s="5"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="23"/>
+      <c r="B178" s="2"/>
+      <c r="C178" s="2"/>
+      <c r="D178" s="2"/>
+      <c r="E178" s="5"/>
+    </row>
+    <row r="179" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="24"/>
+      <c r="B179" s="7"/>
+      <c r="C179" s="7"/>
+      <c r="D179" s="7"/>
+      <c r="E179" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
My scene + planning
</commit_message>
<xml_diff>
--- a/Documentation/Asset list & planning.xlsx
+++ b/Documentation/Asset list & planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="380">
   <si>
     <t>Probation Area</t>
   </si>
@@ -1017,9 +1017,6 @@
     <t>LaserMaze</t>
   </si>
   <si>
-    <t>ShapePuzzle</t>
-  </si>
-  <si>
     <t>SpotTheDiffrences</t>
   </si>
   <si>
@@ -1057,9 +1054,6 @@
   </si>
   <si>
     <t>ConversationController.cs</t>
-  </si>
-  <si>
-    <t>ShapePuzzle.cs</t>
   </si>
   <si>
     <t>RushHour.cs</t>
@@ -1889,10 +1883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T224"/>
+  <dimension ref="A1:T223"/>
   <sheetViews>
-    <sheetView topLeftCell="A141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,8 +2015,8 @@
       <c r="E5" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F5" s="38" t="s">
-        <v>284</v>
+      <c r="F5" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="2"/>
@@ -2055,8 +2049,8 @@
       <c r="E6" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F6" s="38" t="s">
-        <v>284</v>
+      <c r="F6" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="2"/>
@@ -2123,8 +2117,8 @@
       <c r="E8" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F8" s="38" t="s">
-        <v>284</v>
+      <c r="F8" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="2"/>
@@ -2257,8 +2251,8 @@
       <c r="E12" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="F12" s="38" t="s">
-        <v>284</v>
+      <c r="F12" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="2"/>
@@ -2323,8 +2317,8 @@
       <c r="E14" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="F14" s="38" t="s">
-        <v>284</v>
+      <c r="F14" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="2"/>
@@ -2389,8 +2383,8 @@
       <c r="E16" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="F16" s="38" t="s">
-        <v>284</v>
+      <c r="F16" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="2"/>
@@ -2417,8 +2411,8 @@
       <c r="E17" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F17" s="38" t="s">
-        <v>284</v>
+      <c r="F17" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>109</v>
@@ -2449,8 +2443,8 @@
       <c r="E18" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F18" s="38" t="s">
-        <v>284</v>
+      <c r="F18" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="2"/>
@@ -2511,8 +2505,8 @@
       <c r="E20" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F20" s="38" t="s">
-        <v>284</v>
+      <c r="F20" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="2"/>
@@ -2543,8 +2537,8 @@
       <c r="E21" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F21" s="38" t="s">
-        <v>284</v>
+      <c r="F21" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="2"/>
@@ -2575,8 +2569,8 @@
       <c r="E22" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F22" s="38" t="s">
-        <v>284</v>
+      <c r="F22" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="2"/>
@@ -2605,8 +2599,8 @@
       <c r="E23" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F23" s="38" t="s">
-        <v>284</v>
+      <c r="F23" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="2"/>
@@ -2635,8 +2629,8 @@
       <c r="E24" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F24" s="38" t="s">
-        <v>284</v>
+      <c r="F24" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="2"/>
@@ -2665,8 +2659,8 @@
       <c r="E25" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F25" s="38" t="s">
-        <v>284</v>
+      <c r="F25" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="2"/>
@@ -4858,10 +4852,10 @@
       <c r="A130" s="14"/>
       <c r="B130" s="1"/>
       <c r="C130" s="9" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
@@ -4871,10 +4865,10 @@
       <c r="A131" s="14"/>
       <c r="B131" s="1"/>
       <c r="C131" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
@@ -4884,10 +4878,10 @@
       <c r="A132" s="14"/>
       <c r="B132" s="1"/>
       <c r="C132" s="9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
@@ -4897,10 +4891,10 @@
       <c r="A133" s="14"/>
       <c r="B133" s="1"/>
       <c r="C133" s="9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
@@ -4910,10 +4904,10 @@
       <c r="A134" s="14"/>
       <c r="B134" s="1"/>
       <c r="C134" s="9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
@@ -4923,10 +4917,10 @@
       <c r="A135" s="14"/>
       <c r="B135" s="1"/>
       <c r="C135" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
@@ -4936,10 +4930,10 @@
       <c r="A136" s="14"/>
       <c r="B136" s="1"/>
       <c r="C136" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
@@ -4966,10 +4960,10 @@
       <c r="A138" s="14"/>
       <c r="B138" s="1"/>
       <c r="C138" s="9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D138" s="9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138" s="2"/>
@@ -4979,10 +4973,10 @@
       <c r="A139" s="14"/>
       <c r="B139" s="1"/>
       <c r="C139" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
@@ -4992,10 +4986,10 @@
       <c r="A140" s="14"/>
       <c r="B140" s="1"/>
       <c r="C140" s="9" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E140" s="2"/>
       <c r="F140" s="2"/>
@@ -5005,10 +4999,10 @@
       <c r="A141" s="14"/>
       <c r="B141" s="1"/>
       <c r="C141" s="9" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
@@ -5018,10 +5012,10 @@
       <c r="A142" s="14"/>
       <c r="B142" s="1"/>
       <c r="C142" s="9" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D142" s="9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
@@ -5031,10 +5025,10 @@
       <c r="A143" s="14"/>
       <c r="B143" s="1"/>
       <c r="C143" s="9" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
@@ -5298,10 +5292,10 @@
       <c r="A164" s="14"/>
       <c r="B164" s="6"/>
       <c r="C164" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D164" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E164" s="7"/>
       <c r="F164" s="7"/>
@@ -5695,7 +5689,7 @@
         <v>17</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>282</v>
@@ -5723,8 +5717,8 @@
       <c r="D199" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E199" s="38" t="s">
-        <v>284</v>
+      <c r="E199" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="F199" s="5"/>
     </row>
@@ -5737,8 +5731,8 @@
       <c r="D200" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E200" s="38" t="s">
-        <v>284</v>
+      <c r="E200" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="F200" s="5"/>
     </row>
@@ -5760,7 +5754,7 @@
       <c r="A202" s="13"/>
       <c r="B202" s="23"/>
       <c r="C202" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D202" s="9" t="s">
         <v>289</v>
@@ -5845,8 +5839,8 @@
       <c r="D208" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E208" s="38" t="s">
-        <v>284</v>
+      <c r="E208" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="F208" s="5"/>
     </row>
@@ -5868,7 +5862,7 @@
       <c r="A210" s="13"/>
       <c r="B210" s="23"/>
       <c r="C210" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D210" s="9" t="s">
         <v>289</v>
@@ -5936,51 +5930,51 @@
       <c r="C215" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D215" s="9" t="s">
+      <c r="D215" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E215" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="F215" s="5"/>
+    </row>
+    <row r="216" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="13"/>
+      <c r="B216" s="24"/>
+      <c r="C216" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D216" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="E215" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="F215" s="5"/>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" s="13"/>
-      <c r="B216" s="23"/>
-      <c r="C216" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D216" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="E216" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="F216" s="5"/>
-    </row>
-    <row r="217" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F216" s="8"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="13"/>
-      <c r="B217" s="24"/>
-      <c r="C217" s="7" t="s">
+      <c r="B217" s="25" t="s">
         <v>332</v>
       </c>
-      <c r="D217" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="E217" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="F217" s="8"/>
+      <c r="C217" s="3"/>
+      <c r="D217" s="3"/>
+      <c r="E217" s="3"/>
+      <c r="F217" s="4"/>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="13"/>
-      <c r="B218" s="25" t="s">
+      <c r="B218" s="23"/>
+      <c r="C218" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C218" s="3"/>
-      <c r="D218" s="3"/>
-      <c r="E218" s="3"/>
-      <c r="F218" s="4"/>
+      <c r="D218" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E218" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="F218" s="5"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="13"/>
@@ -5988,8 +5982,8 @@
       <c r="C219" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="D219" s="2" t="s">
-        <v>289</v>
+      <c r="D219" s="9" t="s">
+        <v>288</v>
       </c>
       <c r="E219" s="38" t="s">
         <v>284</v>
@@ -6003,7 +5997,7 @@
         <v>335</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E220" s="38" t="s">
         <v>284</v>
@@ -6017,7 +6011,7 @@
         <v>336</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E221" s="38" t="s">
         <v>284</v>
@@ -6027,44 +6021,30 @@
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="13"/>
       <c r="B222" s="23"/>
-      <c r="C222" s="2" t="s">
+      <c r="C222" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="D222" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E222" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="F222" s="5"/>
+    </row>
+    <row r="223" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A223" s="15"/>
+      <c r="B223" s="24"/>
+      <c r="C223" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="D222" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="E222" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="F222" s="5"/>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" s="13"/>
-      <c r="B223" s="23"/>
-      <c r="C223" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="D223" s="2" t="s">
+      <c r="D223" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="E223" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="F223" s="5"/>
-    </row>
-    <row r="224" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="15"/>
-      <c r="B224" s="24"/>
-      <c r="C224" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="D224" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="E224" s="51" t="s">
-        <v>284</v>
-      </c>
-      <c r="F224" s="8"/>
+      <c r="E223" s="51" t="s">
+        <v>284</v>
+      </c>
+      <c r="F223" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6076,8 +6056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6145,13 +6125,13 @@
         <v>281</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="G2" s="39"/>
       <c r="H2" s="44"/>
@@ -6167,9 +6147,7 @@
       </c>
       <c r="C3" s="41"/>
       <c r="D3" s="45"/>
-      <c r="E3" s="41" t="s">
-        <v>335</v>
-      </c>
+      <c r="E3" s="41"/>
       <c r="G3" s="41"/>
       <c r="H3" s="45"/>
       <c r="I3" s="41"/>
@@ -6240,10 +6218,10 @@
         <v>309</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F8" s="40" t="s">
         <v>322</v>
@@ -6252,10 +6230,10 @@
         <v>321</v>
       </c>
       <c r="H8" s="44" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I8" s="40" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J8" s="44" t="s">
         <v>326</v>
@@ -6278,7 +6256,7 @@
       <c r="G9" s="41"/>
       <c r="H9" s="45"/>
       <c r="I9" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J9" s="45"/>
       <c r="K9" s="41"/>
@@ -6348,22 +6326,22 @@
         <v>297</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D14" s="45" t="s">
+        <v>347</v>
+      </c>
+      <c r="E14" s="41" t="s">
         <v>349</v>
       </c>
-      <c r="E14" s="41" t="s">
-        <v>351</v>
-      </c>
       <c r="F14" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="G14" s="49" t="s">
         <v>350</v>
       </c>
-      <c r="G14" s="49" t="s">
-        <v>352</v>
-      </c>
       <c r="H14" s="45" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="I14" s="41"/>
       <c r="J14" s="45"/>
@@ -6390,7 +6368,7 @@
     <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="54" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="45"/>
@@ -6449,19 +6427,19 @@
         <v>299</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F20" s="40" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G20" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H20" s="44"/>
       <c r="I20" s="39"/>

</xml_diff>

<commit_message>
Deleted no name empty materials :C
</commit_message>
<xml_diff>
--- a/Documentation/Asset list & planning.xlsx
+++ b/Documentation/Asset list & planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1890,7 +1890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
@@ -6071,8 +6071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
My stuff and a shitload of meta
</commit_message>
<xml_diff>
--- a/Documentation/Asset list & planning.xlsx
+++ b/Documentation/Asset list & planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1894,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T222"/>
   <sheetViews>
-    <sheetView topLeftCell="B46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="B36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3726,8 +3726,8 @@
       <c r="E61" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F61" s="38" t="s">
-        <v>284</v>
+      <c r="F61" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="2"/>
@@ -3838,7 +3838,7 @@
         <v>153</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="F65" s="38" t="s">
         <v>284</v>
@@ -3924,8 +3924,8 @@
       <c r="E68" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F68" s="38" t="s">
-        <v>284</v>
+      <c r="F68" s="37" t="s">
+        <v>283</v>
       </c>
       <c r="G68" s="5"/>
       <c r="H68" s="2"/>
@@ -6059,7 +6059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Assetlist area 2 update
</commit_message>
<xml_diff>
--- a/Documentation/Asset list & planning.xlsx
+++ b/Documentation/Asset list & planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="401">
   <si>
     <t>Probation Area</t>
   </si>
@@ -1180,6 +1180,54 @@
   </si>
   <si>
     <t>Level design - Storage</t>
+  </si>
+  <si>
+    <t>Brick Furnace</t>
+  </si>
+  <si>
+    <t>Freezer</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Pans</t>
+  </si>
+  <si>
+    <t>Fire extinguisher</t>
+  </si>
+  <si>
+    <t>Kitchen counter</t>
+  </si>
+  <si>
+    <t>Large meat piece</t>
+  </si>
+  <si>
+    <t>Bottles</t>
+  </si>
+  <si>
+    <t>3D_ENV_KITCH_BrickFurnace</t>
+  </si>
+  <si>
+    <t>3D_ENV_KITCH_Freezer</t>
+  </si>
+  <si>
+    <t>3D_ENV_KITCH_Refrigerator</t>
+  </si>
+  <si>
+    <t>3D_ENV_KITCH_Pans</t>
+  </si>
+  <si>
+    <t>3D_ENV_KITCH_Bottles</t>
+  </si>
+  <si>
+    <t>3D_ENV_KITCH_FireExtinguisher</t>
+  </si>
+  <si>
+    <t>3D_ENV_KITCH_KitchenCounter</t>
+  </si>
+  <si>
+    <t>3D_ENV_KITCH_LargeMeat</t>
   </si>
 </sst>
 </file>
@@ -1858,10 +1906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T222"/>
+  <dimension ref="A1:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D225" sqref="D225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4283,8 +4331,12 @@
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="14"/>
       <c r="B87" s="1"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
+      <c r="C87" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>393</v>
+      </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="5"/>
@@ -4292,8 +4344,12 @@
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="14"/>
       <c r="B88" s="1"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
+      <c r="C88" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>394</v>
+      </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="5"/>
@@ -4301,102 +4357,100 @@
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="14"/>
       <c r="B89" s="1"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
+      <c r="C89" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>395</v>
+      </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="14"/>
-      <c r="B90" s="6"/>
-      <c r="C90" s="7"/>
-      <c r="D90" s="7"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="7"/>
-      <c r="G90" s="8"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="5"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="14"/>
-      <c r="B91" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="4"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="5"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="14"/>
       <c r="B92" s="1"/>
-      <c r="C92" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>232</v>
-      </c>
+      <c r="C92" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="5"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
       <c r="B93" s="1"/>
-      <c r="C93" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="F93" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="G93" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C93" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="5"/>
+    </row>
+    <row r="94" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="14"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="F94" s="2"/>
-      <c r="G94" s="5"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="8"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="14"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="F95" s="2"/>
-      <c r="G95" s="5"/>
+      <c r="B95" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="4"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="14"/>
       <c r="B96" s="1"/>
-      <c r="C96" s="9" t="s">
-        <v>48</v>
+      <c r="C96" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>232</v>
@@ -4407,12 +4461,12 @@
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="14"/>
       <c r="B97" s="1"/>
-      <c r="C97" s="9" t="s">
-        <v>49</v>
+      <c r="C97" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2" t="s">
-        <v>138</v>
+        <v>232</v>
       </c>
       <c r="F97" s="37" t="s">
         <v>282</v>
@@ -4421,45 +4475,47 @@
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="14"/>
       <c r="B98" s="1"/>
-      <c r="C98" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D98" s="2"/>
+      <c r="C98" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="E98" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F98" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="F98" s="2"/>
+      <c r="G98" s="5"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="14"/>
-      <c r="B99" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
-      <c r="G99" s="4"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F99" s="2"/>
+      <c r="G99" s="5"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="14"/>
       <c r="B100" s="1"/>
-      <c r="C100" s="2" t="s">
-        <v>192</v>
+      <c r="C100" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>193</v>
+        <v>89</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="5"/>
@@ -4467,195 +4523,195 @@
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="14"/>
       <c r="B101" s="1"/>
-      <c r="C101" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>98</v>
-      </c>
+      <c r="C101" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D101" s="2"/>
       <c r="E101" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F101" s="2"/>
-      <c r="G101" s="5"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="F101" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="14"/>
       <c r="B102" s="1"/>
-      <c r="C102" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>100</v>
-      </c>
+      <c r="C102" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D102" s="2"/>
       <c r="E102" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F102" s="2"/>
-      <c r="G102" s="5"/>
+        <v>138</v>
+      </c>
+      <c r="F102" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="14"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F103" s="2"/>
-      <c r="G103" s="5"/>
+      <c r="B103" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="4"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
       <c r="B104" s="1"/>
-      <c r="C104" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D104" s="9" t="s">
-        <v>101</v>
+      <c r="C104" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="F104" s="9"/>
+        <v>207</v>
+      </c>
+      <c r="F104" s="2"/>
       <c r="G104" s="5"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="14"/>
       <c r="B105" s="1"/>
-      <c r="C105" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D105" s="9" t="s">
-        <v>236</v>
+      <c r="C105" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F105" s="9"/>
+      <c r="F105" s="2"/>
       <c r="G105" s="5"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="14"/>
       <c r="B106" s="1"/>
-      <c r="C106" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="D106" s="9" t="s">
-        <v>237</v>
+      <c r="C106" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F106" s="9"/>
+      <c r="F106" s="2"/>
       <c r="G106" s="5"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="14"/>
       <c r="B107" s="1"/>
-      <c r="C107" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D107" s="9"/>
-      <c r="E107" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F107" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="G107" s="5" t="s">
-        <v>109</v>
-      </c>
+      <c r="C107" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F107" s="2"/>
+      <c r="G107" s="5"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="14"/>
       <c r="B108" s="1"/>
       <c r="C108" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="D108" s="9"/>
-      <c r="E108" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="F108" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="G108" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F108" s="9"/>
+      <c r="G108" s="5"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="14"/>
       <c r="B109" s="1"/>
       <c r="C109" s="9" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="E109" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="E109" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F109" s="2"/>
+      <c r="F109" s="9"/>
       <c r="G109" s="5"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="14"/>
       <c r="B110" s="1"/>
       <c r="C110" s="9" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="E110" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="E110" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F110" s="2"/>
+      <c r="F110" s="9"/>
       <c r="G110" s="5"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="14"/>
       <c r="B111" s="1"/>
       <c r="C111" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="D111" s="9" t="s">
-        <v>259</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D111" s="9"/>
       <c r="E111" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="F111" s="2"/>
-      <c r="G111" s="5"/>
-    </row>
-    <row r="112" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="F111" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="G111" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="14"/>
       <c r="B112" s="1"/>
       <c r="C112" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="D112" s="33" t="s">
-        <v>260</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="D112" s="9"/>
       <c r="E112" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="F112" s="2"/>
-      <c r="G112" s="5"/>
-    </row>
-    <row r="113" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="F112" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="G112" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="14"/>
       <c r="B113" s="1"/>
       <c r="C113" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="D113" s="33" t="s">
-        <v>261</v>
+        <v>238</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>254</v>
       </c>
       <c r="E113" s="9" t="s">
         <v>207</v>
@@ -4663,14 +4719,14 @@
       <c r="F113" s="2"/>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
       <c r="B114" s="1"/>
       <c r="C114" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="D114" s="33" t="s">
-        <v>256</v>
+        <v>239</v>
+      </c>
+      <c r="D114" s="9" t="s">
+        <v>255</v>
       </c>
       <c r="E114" s="9" t="s">
         <v>207</v>
@@ -4678,14 +4734,14 @@
       <c r="F114" s="2"/>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="14"/>
       <c r="B115" s="1"/>
       <c r="C115" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="D115" s="33" t="s">
-        <v>262</v>
+        <v>240</v>
+      </c>
+      <c r="D115" s="9" t="s">
+        <v>259</v>
       </c>
       <c r="E115" s="9" t="s">
         <v>207</v>
@@ -4697,10 +4753,10 @@
       <c r="A116" s="14"/>
       <c r="B116" s="1"/>
       <c r="C116" s="9" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D116" s="33" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E116" s="9" t="s">
         <v>207</v>
@@ -4712,10 +4768,10 @@
       <c r="A117" s="14"/>
       <c r="B117" s="1"/>
       <c r="C117" s="9" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="D117" s="33" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>207</v>
@@ -4727,25 +4783,25 @@
       <c r="A118" s="14"/>
       <c r="B118" s="1"/>
       <c r="C118" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="D118" s="33"/>
+        <v>243</v>
+      </c>
+      <c r="D118" s="33" t="s">
+        <v>256</v>
+      </c>
       <c r="E118" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="F118" s="37" t="s">
-        <v>282</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="F118" s="2"/>
       <c r="G118" s="5"/>
     </row>
     <row r="119" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
       <c r="B119" s="1"/>
       <c r="C119" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D119" s="34" t="s">
-        <v>266</v>
+        <v>244</v>
+      </c>
+      <c r="D119" s="33" t="s">
+        <v>262</v>
       </c>
       <c r="E119" s="9" t="s">
         <v>207</v>
@@ -4757,10 +4813,10 @@
       <c r="A120" s="14"/>
       <c r="B120" s="1"/>
       <c r="C120" s="9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D120" s="33" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>207</v>
@@ -4772,13 +4828,13 @@
       <c r="A121" s="14"/>
       <c r="B121" s="1"/>
       <c r="C121" s="9" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="D121" s="33" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="E121" s="9" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="F121" s="2"/>
       <c r="G121" s="5"/>
@@ -4787,25 +4843,25 @@
       <c r="A122" s="14"/>
       <c r="B122" s="1"/>
       <c r="C122" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="D122" s="33" t="s">
-        <v>258</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="D122" s="33"/>
       <c r="E122" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="F122" s="2"/>
+        <v>210</v>
+      </c>
+      <c r="F122" s="37" t="s">
+        <v>282</v>
+      </c>
       <c r="G122" s="5"/>
     </row>
     <row r="123" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
       <c r="B123" s="1"/>
       <c r="C123" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="D123" s="33" t="s">
-        <v>268</v>
+        <v>247</v>
+      </c>
+      <c r="D123" s="34" t="s">
+        <v>266</v>
       </c>
       <c r="E123" s="9" t="s">
         <v>207</v>
@@ -4817,10 +4873,10 @@
       <c r="A124" s="14"/>
       <c r="B124" s="1"/>
       <c r="C124" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="D124" s="35" t="s">
-        <v>269</v>
+        <v>248</v>
+      </c>
+      <c r="D124" s="33" t="s">
+        <v>267</v>
       </c>
       <c r="E124" s="9" t="s">
         <v>207</v>
@@ -4832,105 +4888,105 @@
       <c r="A125" s="14"/>
       <c r="B125" s="1"/>
       <c r="C125" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="D125" s="36" t="s">
-        <v>270</v>
+        <v>249</v>
+      </c>
+      <c r="D125" s="33" t="s">
+        <v>257</v>
       </c>
       <c r="E125" s="9" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="F125" s="2"/>
       <c r="G125" s="5"/>
     </row>
-    <row r="126" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="14"/>
-      <c r="B126" s="6"/>
-      <c r="C126" s="7"/>
-      <c r="D126" s="7"/>
-      <c r="E126" s="7"/>
-      <c r="F126" s="7"/>
-      <c r="G126" s="8"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B126" s="1"/>
+      <c r="C126" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D126" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="E126" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="F126" s="2"/>
+      <c r="G126" s="5"/>
+    </row>
+    <row r="127" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="14"/>
-      <c r="B127" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
-      <c r="E127" s="3"/>
-      <c r="F127" s="3"/>
-      <c r="G127" s="4"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B127" s="1"/>
+      <c r="C127" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D127" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="E127" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="F127" s="2"/>
+      <c r="G127" s="5"/>
+    </row>
+    <row r="128" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="14"/>
       <c r="B128" s="1"/>
-      <c r="C128" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>194</v>
+      <c r="C128" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D128" s="35" t="s">
+        <v>269</v>
       </c>
       <c r="E128" s="9" t="s">
-        <v>138</v>
+        <v>207</v>
       </c>
       <c r="F128" s="2"/>
       <c r="G128" s="5"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="14"/>
       <c r="B129" s="1"/>
       <c r="C129" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="D129" s="9" t="s">
-        <v>376</v>
+        <v>253</v>
+      </c>
+      <c r="D129" s="36" t="s">
+        <v>270</v>
       </c>
       <c r="E129" s="9" t="s">
-        <v>138</v>
+        <v>207</v>
       </c>
       <c r="F129" s="2"/>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="14"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="D130" s="9" t="s">
-        <v>377</v>
-      </c>
-      <c r="E130" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F130" s="2"/>
-      <c r="G130" s="5"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="7"/>
+      <c r="D130" s="7"/>
+      <c r="E130" s="7"/>
+      <c r="F130" s="7"/>
+      <c r="G130" s="8"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="14"/>
-      <c r="B131" s="1"/>
-      <c r="C131" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="D131" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="E131" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F131" s="2"/>
-      <c r="G131" s="5"/>
+      <c r="B131" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="4"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="14"/>
       <c r="B132" s="1"/>
-      <c r="C132" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="D132" s="9" t="s">
-        <v>365</v>
+      <c r="C132" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="E132" s="9" t="s">
         <v>138</v>
@@ -4942,10 +4998,10 @@
       <c r="A133" s="14"/>
       <c r="B133" s="1"/>
       <c r="C133" s="9" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="E133" s="9" t="s">
         <v>138</v>
@@ -4957,10 +5013,10 @@
       <c r="A134" s="14"/>
       <c r="B134" s="1"/>
       <c r="C134" s="9" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="E134" s="9" t="s">
         <v>138</v>
@@ -4972,10 +5028,10 @@
       <c r="A135" s="14"/>
       <c r="B135" s="1"/>
       <c r="C135" s="9" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E135" s="9" t="s">
         <v>138</v>
@@ -4987,27 +5043,25 @@
       <c r="A136" s="14"/>
       <c r="B136" s="1"/>
       <c r="C136" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D136" s="2"/>
-      <c r="E136" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F136" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="G136" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="D136" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="E136" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F136" s="2"/>
+      <c r="G136" s="5"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="14"/>
       <c r="B137" s="1"/>
       <c r="C137" s="9" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E137" s="9" t="s">
         <v>138</v>
@@ -5019,10 +5073,10 @@
       <c r="A138" s="14"/>
       <c r="B138" s="1"/>
       <c r="C138" s="9" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D138" s="9" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E138" s="9" t="s">
         <v>138</v>
@@ -5034,10 +5088,10 @@
       <c r="A139" s="14"/>
       <c r="B139" s="1"/>
       <c r="C139" s="9" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="E139" s="9" t="s">
         <v>138</v>
@@ -5049,25 +5103,27 @@
       <c r="A140" s="14"/>
       <c r="B140" s="1"/>
       <c r="C140" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="D140" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="E140" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="F140" s="2"/>
-      <c r="G140" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F140" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="G140" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="14"/>
       <c r="B141" s="1"/>
       <c r="C141" s="9" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E141" s="9" t="s">
         <v>138</v>
@@ -5079,10 +5135,10 @@
       <c r="A142" s="14"/>
       <c r="B142" s="1"/>
       <c r="C142" s="9" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D142" s="9" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E142" s="9" t="s">
         <v>138</v>
@@ -5093,210 +5149,224 @@
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="14"/>
       <c r="B143" s="1"/>
-      <c r="C143" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2" t="s">
+      <c r="C143" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="D143" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="E143" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F143" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="G143" s="5" t="s">
-        <v>109</v>
-      </c>
+      <c r="F143" s="2"/>
+      <c r="G143" s="5"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
       <c r="B144" s="1"/>
-      <c r="C144" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D144" s="2"/>
-      <c r="E144" s="2" t="s">
+      <c r="C144" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="D144" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="E144" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F144" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="G144" s="5" t="s">
-        <v>109</v>
-      </c>
+      <c r="F144" s="2"/>
+      <c r="G144" s="5"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="14"/>
       <c r="B145" s="1"/>
-      <c r="C145" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E145" s="2" t="s">
+      <c r="C145" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="D145" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="E145" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F145" s="37" t="s">
-        <v>282</v>
-      </c>
+      <c r="F145" s="2"/>
       <c r="G145" s="5"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="14"/>
       <c r="B146" s="1"/>
       <c r="C146" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E146" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D146" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="E146" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F146" s="37" t="s">
-        <v>282</v>
-      </c>
+      <c r="F146" s="2"/>
       <c r="G146" s="5"/>
     </row>
-    <row r="147" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="14"/>
       <c r="B147" s="1"/>
-      <c r="C147" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E147" s="9" t="s">
+      <c r="C147" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2" t="s">
         <v>138</v>
       </c>
       <c r="F147" s="37" t="s">
         <v>282</v>
       </c>
-      <c r="G147" s="5"/>
+      <c r="G147" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="14"/>
-      <c r="B148" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C148" s="3"/>
-      <c r="D148" s="3"/>
-      <c r="E148" s="3"/>
-      <c r="F148" s="3"/>
-      <c r="G148" s="4"/>
+      <c r="B148" s="1"/>
+      <c r="C148" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D148" s="2"/>
+      <c r="E148" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F148" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="G148" s="5" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="14"/>
       <c r="B149" s="1"/>
-      <c r="C149" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D149" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="E149" s="2"/>
-      <c r="F149" s="2"/>
+      <c r="C149" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F149" s="37" t="s">
+        <v>282</v>
+      </c>
       <c r="G149" s="5"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="14"/>
       <c r="B150" s="1"/>
       <c r="C150" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D150" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="E150" s="2"/>
-      <c r="F150" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F150" s="37" t="s">
+        <v>282</v>
+      </c>
       <c r="G150" s="5"/>
     </row>
     <row r="151" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="15"/>
-      <c r="B151" s="6"/>
-      <c r="C151" s="7"/>
-      <c r="D151" s="7"/>
-      <c r="E151" s="7"/>
-      <c r="F151" s="7"/>
-      <c r="G151" s="8"/>
-    </row>
-    <row r="152" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="9"/>
-      <c r="B152" s="9"/>
-      <c r="C152" s="9"/>
-      <c r="D152" s="9"/>
-      <c r="E152" s="9"/>
-      <c r="F152" s="9"/>
-      <c r="G152" s="9"/>
-    </row>
-    <row r="153" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B153" s="3"/>
-      <c r="C153" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E153" s="3"/>
-      <c r="F153" s="3"/>
-      <c r="G153" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A151" s="14"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E151" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F151" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="G151" s="5"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="14"/>
+      <c r="B152" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C152" s="3"/>
+      <c r="D152" s="3"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3"/>
+      <c r="G152" s="4"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="14"/>
+      <c r="B153" s="1"/>
+      <c r="C153" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D153" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="5"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="14"/>
-      <c r="B154" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C154" s="3"/>
-      <c r="D154" s="3"/>
-      <c r="E154" s="3"/>
-      <c r="F154" s="3"/>
-      <c r="G154" s="4"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="14"/>
-      <c r="B155" s="1"/>
-      <c r="C155" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D155" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E155" s="2"/>
-      <c r="F155" s="2"/>
-      <c r="G155" s="5"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A156" s="14"/>
-      <c r="B156" s="1"/>
-      <c r="C156" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E156" s="2"/>
-      <c r="F156" s="2"/>
-      <c r="G156" s="5"/>
+      <c r="B154" s="1"/>
+      <c r="C154" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D154" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="5"/>
+    </row>
+    <row r="155" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="15"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="7"/>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
+      <c r="F155" s="7"/>
+      <c r="G155" s="8"/>
+    </row>
+    <row r="156" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="9"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
     </row>
     <row r="157" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="14"/>
-      <c r="B157" s="6"/>
-      <c r="C157" s="7"/>
-      <c r="D157" s="7"/>
-      <c r="E157" s="7"/>
-      <c r="F157" s="7"/>
-      <c r="G157" s="8"/>
+      <c r="A157" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B157" s="3"/>
+      <c r="C157" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="14"/>
       <c r="B158" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
@@ -5308,294 +5378,276 @@
       <c r="A159" s="14"/>
       <c r="B159" s="1"/>
       <c r="C159" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E159" s="2"/>
       <c r="F159" s="2"/>
       <c r="G159" s="5"/>
     </row>
-    <row r="160" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="14"/>
-      <c r="B160" s="6"/>
-      <c r="C160" s="7"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="7"/>
-      <c r="F160" s="7"/>
-      <c r="G160" s="8"/>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B160" s="1"/>
+      <c r="C160" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="5"/>
+    </row>
+    <row r="161" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="14"/>
-      <c r="B161" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C161" s="3"/>
-      <c r="D161" s="3"/>
-      <c r="E161" s="3"/>
-      <c r="F161" s="3"/>
-      <c r="G161" s="4"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="7"/>
+      <c r="D161" s="7"/>
+      <c r="E161" s="7"/>
+      <c r="F161" s="7"/>
+      <c r="G161" s="8"/>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="14"/>
-      <c r="B162" s="1"/>
-      <c r="C162" s="2" t="s">
+      <c r="B162" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C162" s="3"/>
+      <c r="D162" s="3"/>
+      <c r="E162" s="3"/>
+      <c r="F162" s="3"/>
+      <c r="G162" s="4"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="14"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E163" s="2"/>
+      <c r="F163" s="2"/>
+      <c r="G163" s="5"/>
+    </row>
+    <row r="164" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="14"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="7"/>
+      <c r="D164" s="7"/>
+      <c r="E164" s="7"/>
+      <c r="F164" s="7"/>
+      <c r="G164" s="8"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="14"/>
+      <c r="B165" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C165" s="3"/>
+      <c r="D165" s="3"/>
+      <c r="E165" s="3"/>
+      <c r="F165" s="3"/>
+      <c r="G165" s="4"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="14"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D162" s="2" t="s">
+      <c r="D166" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E162" s="2"/>
-      <c r="F162" s="2"/>
-      <c r="G162" s="5"/>
-    </row>
-    <row r="163" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="14"/>
-      <c r="B163" s="6"/>
-      <c r="C163" s="7" t="s">
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="5"/>
+    </row>
+    <row r="167" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="14"/>
+      <c r="B167" s="6"/>
+      <c r="C167" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="D163" s="7" t="s">
+      <c r="D167" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="E163" s="7"/>
-      <c r="F163" s="7"/>
-      <c r="G163" s="8"/>
-    </row>
-    <row r="164" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="22"/>
-      <c r="B164" s="25" t="s">
+      <c r="E167" s="7"/>
+      <c r="F167" s="7"/>
+      <c r="G167" s="8"/>
+    </row>
+    <row r="168" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="22"/>
+      <c r="B168" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C164" s="3"/>
-      <c r="D164" s="3"/>
-      <c r="E164" s="3"/>
-      <c r="F164" s="3"/>
-      <c r="G164" s="4"/>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A165" s="20"/>
-      <c r="B165" s="30"/>
-      <c r="C165" s="9" t="s">
+      <c r="C168" s="3"/>
+      <c r="D168" s="3"/>
+      <c r="E168" s="3"/>
+      <c r="F168" s="3"/>
+      <c r="G168" s="4"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="20"/>
+      <c r="B169" s="30"/>
+      <c r="C169" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="D165" s="9" t="s">
+      <c r="D169" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="E165" s="9"/>
-      <c r="F165" s="9"/>
-      <c r="G165" s="26"/>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A166" s="20"/>
-      <c r="B166" s="23"/>
-      <c r="C166" s="9"/>
-      <c r="D166" s="9"/>
-      <c r="E166" s="9"/>
-      <c r="F166" s="9"/>
-      <c r="G166" s="26"/>
-    </row>
-    <row r="167" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="21"/>
-      <c r="B167" s="24"/>
-      <c r="C167" s="17"/>
-      <c r="D167" s="17"/>
-      <c r="E167" s="17"/>
-      <c r="F167" s="17"/>
-      <c r="G167" s="18"/>
-    </row>
-    <row r="168" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="9"/>
-      <c r="B168" s="9"/>
-      <c r="C168" s="9"/>
-      <c r="D168" s="9"/>
-      <c r="E168" s="9"/>
-      <c r="F168" s="9"/>
-      <c r="G168" s="9"/>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" s="31" t="s">
+      <c r="E169" s="9"/>
+      <c r="F169" s="9"/>
+      <c r="G169" s="26"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="20"/>
+      <c r="B170" s="23"/>
+      <c r="C170" s="9"/>
+      <c r="D170" s="9"/>
+      <c r="E170" s="9"/>
+      <c r="F170" s="9"/>
+      <c r="G170" s="26"/>
+    </row>
+    <row r="171" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="21"/>
+      <c r="B171" s="24"/>
+      <c r="C171" s="17"/>
+      <c r="D171" s="17"/>
+      <c r="E171" s="17"/>
+      <c r="F171" s="17"/>
+      <c r="G171" s="18"/>
+    </row>
+    <row r="172" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="9"/>
+      <c r="B172" s="9"/>
+      <c r="C172" s="9"/>
+      <c r="D172" s="9"/>
+      <c r="E172" s="9"/>
+      <c r="F172" s="9"/>
+      <c r="G172" s="9"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="B169" s="28"/>
-      <c r="C169" s="28"/>
-      <c r="D169" s="28"/>
-      <c r="E169" s="29"/>
-      <c r="F169" s="9"/>
-    </row>
-    <row r="170" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A170" s="32"/>
-      <c r="B170" s="9" t="s">
+      <c r="B173" s="28"/>
+      <c r="C173" s="28"/>
+      <c r="D173" s="28"/>
+      <c r="E173" s="29"/>
+      <c r="F173" s="9"/>
+    </row>
+    <row r="174" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A174" s="32"/>
+      <c r="B174" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C170" s="9" t="s">
+      <c r="C174" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="D170" s="9"/>
-      <c r="E170" s="26"/>
-      <c r="F170" s="9"/>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A171" s="23"/>
-      <c r="B171" s="9"/>
-      <c r="C171" s="9"/>
-      <c r="D171" s="9"/>
-      <c r="E171" s="26"/>
-      <c r="F171" s="9"/>
-    </row>
-    <row r="172" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="24"/>
-      <c r="B172" s="17"/>
-      <c r="C172" s="17"/>
-      <c r="D172" s="17"/>
-      <c r="E172" s="18"/>
-      <c r="F172" s="9"/>
-    </row>
-    <row r="173" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A174" s="25" t="s">
+      <c r="D174" s="9"/>
+      <c r="E174" s="26"/>
+      <c r="F174" s="9"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="23"/>
+      <c r="B175" s="9"/>
+      <c r="C175" s="9"/>
+      <c r="D175" s="9"/>
+      <c r="E175" s="26"/>
+      <c r="F175" s="9"/>
+    </row>
+    <row r="176" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="24"/>
+      <c r="B176" s="17"/>
+      <c r="C176" s="17"/>
+      <c r="D176" s="17"/>
+      <c r="E176" s="18"/>
+      <c r="F176" s="9"/>
+    </row>
+    <row r="177" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="B174" s="25" t="s">
+      <c r="B178" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C174" s="3" t="s">
+      <c r="C178" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D174" s="3" t="s">
+      <c r="D178" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E174" s="3" t="s">
+      <c r="E178" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="F174" s="4" t="s">
+      <c r="F178" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G174" s="2"/>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A175" s="52"/>
-      <c r="B175" s="22" t="s">
+      <c r="G178" s="2"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="52"/>
+      <c r="B179" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C179" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="D175" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E175" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="F175" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="G175" s="2"/>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A176" s="52"/>
-      <c r="B176" s="22" t="s">
-        <v>311</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E176" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="F176" s="5"/>
-      <c r="G176" s="2"/>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A177" s="23"/>
-      <c r="B177" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D177" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E177" s="9"/>
-      <c r="F177" s="5"/>
-      <c r="G177" s="2"/>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A178" s="23"/>
-      <c r="B178" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D178" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E178" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="F178" s="5"/>
-      <c r="G178" s="2"/>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" s="23"/>
-      <c r="B179" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="C179" s="9" t="s">
-        <v>225</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="E179" s="2"/>
-      <c r="F179" s="5"/>
+      <c r="E179" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="F179" s="5" t="s">
+        <v>314</v>
+      </c>
       <c r="G179" s="2"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" s="23"/>
+      <c r="A180" s="52"/>
       <c r="B180" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="C180" s="9" t="s">
-        <v>224</v>
+        <v>311</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>315</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="E180" s="2"/>
+      <c r="E180" s="38" t="s">
+        <v>283</v>
+      </c>
       <c r="F180" s="5"/>
       <c r="G180" s="2"/>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="23"/>
       <c r="B181" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="C181" s="9" t="s">
-        <v>226</v>
+        <v>212</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="E181" s="38" t="s">
-        <v>283</v>
-      </c>
+      <c r="E181" s="9"/>
       <c r="F181" s="5"/>
       <c r="G181" s="2"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="23"/>
       <c r="B182" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="C182" s="9" t="s">
-        <v>227</v>
+        <v>213</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>313</v>
@@ -5609,10 +5661,10 @@
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="23"/>
       <c r="B183" s="22" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>313</v>
@@ -5624,10 +5676,10 @@
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="23"/>
       <c r="B184" s="22" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>313</v>
@@ -5639,206 +5691,214 @@
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="23"/>
       <c r="B185" s="22" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="E185" s="2"/>
+      <c r="E185" s="38" t="s">
+        <v>283</v>
+      </c>
       <c r="F185" s="5"/>
       <c r="G185" s="2"/>
     </row>
-    <row r="186" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="24"/>
-      <c r="B186" s="53" t="s">
-        <v>221</v>
-      </c>
-      <c r="C186" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="D186" s="7" t="s">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="23"/>
+      <c r="B186" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="C186" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D186" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="E186" s="51" t="s">
+      <c r="E186" s="38" t="s">
         <v>283</v>
       </c>
-      <c r="F186" s="8"/>
+      <c r="F186" s="5"/>
       <c r="G186" s="2"/>
     </row>
-    <row r="187" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="23"/>
+      <c r="B187" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C187" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E187" s="2"/>
+      <c r="F187" s="5"/>
+      <c r="G187" s="2"/>
+    </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" s="25" t="s">
-        <v>272</v>
-      </c>
-      <c r="B188" s="3"/>
-      <c r="C188" s="3"/>
-      <c r="D188" s="3"/>
-      <c r="E188" s="3"/>
-      <c r="F188" s="4"/>
+      <c r="A188" s="23"/>
+      <c r="B188" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C188" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E188" s="2"/>
+      <c r="F188" s="5"/>
+      <c r="G188" s="2"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="23"/>
-      <c r="B189" s="9" t="s">
-        <v>273</v>
+      <c r="B189" s="22" t="s">
+        <v>220</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="D189" s="2"/>
+        <v>230</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>313</v>
+      </c>
       <c r="E189" s="2"/>
       <c r="F189" s="5"/>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A190" s="23"/>
-      <c r="B190" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C190" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="D190" s="2"/>
-      <c r="E190" s="2"/>
-      <c r="F190" s="5"/>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A191" s="23"/>
-      <c r="B191" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="C191" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="D191" s="2"/>
-      <c r="E191" s="2"/>
-      <c r="F191" s="5"/>
-    </row>
+      <c r="G189" s="2"/>
+    </row>
+    <row r="190" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="24"/>
+      <c r="B190" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="C190" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="D190" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="E190" s="51" t="s">
+        <v>283</v>
+      </c>
+      <c r="F190" s="8"/>
+      <c r="G190" s="2"/>
+    </row>
+    <row r="191" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A192" s="23"/>
-      <c r="B192" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="C192" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="D192" s="2"/>
-      <c r="E192" s="2"/>
-      <c r="F192" s="5"/>
+      <c r="A192" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="B192" s="3"/>
+      <c r="C192" s="3"/>
+      <c r="D192" s="3"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="4"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="23"/>
-      <c r="B193" s="2"/>
-      <c r="C193" s="2"/>
+      <c r="B193" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C193" s="9" t="s">
+        <v>276</v>
+      </c>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
       <c r="F193" s="5"/>
     </row>
-    <row r="194" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="24"/>
-      <c r="B194" s="7"/>
-      <c r="C194" s="7"/>
-      <c r="D194" s="7"/>
-      <c r="E194" s="7"/>
-      <c r="F194" s="8"/>
-    </row>
-    <row r="195" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="196" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="16" t="s">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="23"/>
+      <c r="B194" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C194" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D194" s="2"/>
+      <c r="E194" s="2"/>
+      <c r="F194" s="5"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="23"/>
+      <c r="B195" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C195" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="D195" s="2"/>
+      <c r="E195" s="2"/>
+      <c r="F195" s="5"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="23"/>
+      <c r="B196" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C196" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D196" s="2"/>
+      <c r="E196" s="2"/>
+      <c r="F196" s="5"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="23"/>
+      <c r="B197" s="2"/>
+      <c r="C197" s="2"/>
+      <c r="D197" s="2"/>
+      <c r="E197" s="2"/>
+      <c r="F197" s="5"/>
+    </row>
+    <row r="198" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="24"/>
+      <c r="B198" s="7"/>
+      <c r="C198" s="7"/>
+      <c r="D198" s="7"/>
+      <c r="E198" s="7"/>
+      <c r="F198" s="8"/>
+    </row>
+    <row r="199" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="200" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A200" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="B196" s="3"/>
-      <c r="C196" s="3" t="s">
+      <c r="B200" s="3"/>
+      <c r="C200" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D196" s="3" t="s">
+      <c r="D200" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="E196" s="3" t="s">
+      <c r="E200" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="F196" s="29" t="s">
+      <c r="F200" s="29" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" s="13"/>
-      <c r="B197" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="C197" s="3"/>
-      <c r="D197" s="3"/>
-      <c r="E197" s="3"/>
-      <c r="F197" s="4"/>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A198" s="13"/>
-      <c r="B198" s="23"/>
-      <c r="C198" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="D198" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E198" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="F198" s="5"/>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="13"/>
-      <c r="B199" s="23"/>
-      <c r="C199" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="D199" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E199" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="F199" s="5"/>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A200" s="13"/>
-      <c r="B200" s="23"/>
-      <c r="C200" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D200" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="E200" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="F200" s="5"/>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
-      <c r="B201" s="23"/>
-      <c r="C201" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="D201" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="E201" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="F201" s="5"/>
+      <c r="B201" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="C201" s="3"/>
+      <c r="D201" s="3"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="4"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="13"/>
       <c r="B202" s="23"/>
       <c r="C202" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="D202" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="D202" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E202" s="38" t="s">
-        <v>283</v>
+      <c r="E202" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="F202" s="5"/>
     </row>
@@ -5846,13 +5906,13 @@
       <c r="A203" s="13"/>
       <c r="B203" s="23"/>
       <c r="C203" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D203" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="D203" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E203" s="38" t="s">
-        <v>283</v>
+      <c r="E203" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="F203" s="5"/>
     </row>
@@ -5860,7 +5920,7 @@
       <c r="A204" s="13"/>
       <c r="B204" s="23"/>
       <c r="C204" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D204" s="9" t="s">
         <v>288</v>
@@ -5870,13 +5930,13 @@
       </c>
       <c r="F204" s="5"/>
     </row>
-    <row r="205" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="13"/>
       <c r="B205" s="23"/>
-      <c r="C205" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D205" s="2" t="s">
+      <c r="C205" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="D205" s="9" t="s">
         <v>288</v>
       </c>
       <c r="E205" s="38" t="s">
@@ -5886,25 +5946,29 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="13"/>
-      <c r="B206" s="25" t="s">
-        <v>322</v>
-      </c>
-      <c r="C206" s="3"/>
-      <c r="D206" s="3"/>
-      <c r="E206" s="3"/>
-      <c r="F206" s="4"/>
+      <c r="B206" s="23"/>
+      <c r="C206" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D206" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="E206" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="F206" s="5"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
       <c r="B207" s="23"/>
       <c r="C207" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D207" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D207" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="E207" s="37" t="s">
-        <v>282</v>
+      <c r="E207" s="38" t="s">
+        <v>283</v>
       </c>
       <c r="F207" s="5"/>
     </row>
@@ -5912,9 +5976,9 @@
       <c r="A208" s="13"/>
       <c r="B208" s="23"/>
       <c r="C208" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D208" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D208" s="9" t="s">
         <v>288</v>
       </c>
       <c r="E208" s="38" t="s">
@@ -5922,13 +5986,13 @@
       </c>
       <c r="F208" s="5"/>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="13"/>
       <c r="B209" s="23"/>
-      <c r="C209" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="D209" s="9" t="s">
+      <c r="C209" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D209" s="2" t="s">
         <v>288</v>
       </c>
       <c r="E209" s="38" t="s">
@@ -5936,38 +6000,38 @@
       </c>
       <c r="F209" s="5"/>
     </row>
-    <row r="210" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="13"/>
-      <c r="B210" s="24"/>
-      <c r="C210" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="D210" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="E210" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="F210" s="8"/>
+      <c r="B210" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="C210" s="3"/>
+      <c r="D210" s="3"/>
+      <c r="E210" s="3"/>
+      <c r="F210" s="4"/>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="13"/>
-      <c r="B211" s="25" t="s">
-        <v>326</v>
-      </c>
-      <c r="C211" s="3"/>
-      <c r="D211" s="3"/>
-      <c r="E211" s="3"/>
-      <c r="F211" s="4"/>
+      <c r="B211" s="23"/>
+      <c r="C211" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E211" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="F211" s="5"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="13"/>
       <c r="B212" s="23"/>
       <c r="C212" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E212" s="38" t="s">
         <v>283</v>
@@ -5977,63 +6041,63 @@
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="13"/>
       <c r="B213" s="23"/>
-      <c r="C213" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D213" s="2" t="s">
-        <v>289</v>
+      <c r="C213" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="D213" s="9" t="s">
+        <v>288</v>
       </c>
       <c r="E213" s="38" t="s">
         <v>283</v>
       </c>
       <c r="F213" s="5"/>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="13"/>
-      <c r="B214" s="23"/>
-      <c r="C214" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="D214" s="2" t="s">
-        <v>290</v>
+      <c r="B214" s="24"/>
+      <c r="C214" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="D214" s="7" t="s">
+        <v>288</v>
       </c>
       <c r="E214" s="38" t="s">
         <v>283</v>
       </c>
-      <c r="F214" s="5"/>
-    </row>
-    <row r="215" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F214" s="8"/>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
-      <c r="B215" s="24"/>
-      <c r="C215" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="D215" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="E215" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="F215" s="8"/>
+      <c r="B215" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="C215" s="3"/>
+      <c r="D215" s="3"/>
+      <c r="E215" s="3"/>
+      <c r="F215" s="4"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="13"/>
-      <c r="B216" s="25" t="s">
-        <v>331</v>
-      </c>
-      <c r="C216" s="3"/>
-      <c r="D216" s="3"/>
-      <c r="E216" s="3"/>
-      <c r="F216" s="4"/>
+      <c r="B216" s="23"/>
+      <c r="C216" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E216" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="F216" s="5"/>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="13"/>
       <c r="B217" s="23"/>
       <c r="C217" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E217" s="38" t="s">
         <v>283</v>
@@ -6044,71 +6108,123 @@
       <c r="A218" s="13"/>
       <c r="B218" s="23"/>
       <c r="C218" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="D218" s="9" t="s">
-        <v>287</v>
+        <v>329</v>
+      </c>
+      <c r="D218" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="E218" s="38" t="s">
         <v>283</v>
       </c>
       <c r="F218" s="5"/>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="13"/>
-      <c r="B219" s="23"/>
-      <c r="C219" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="D219" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="E219" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="F219" s="5"/>
+      <c r="B219" s="24"/>
+      <c r="C219" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="D219" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E219" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="F219" s="8"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="13"/>
-      <c r="B220" s="23"/>
-      <c r="C220" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="D220" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="E220" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="F220" s="5"/>
+      <c r="B220" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="C220" s="3"/>
+      <c r="D220" s="3"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="4"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="13"/>
       <c r="B221" s="23"/>
-      <c r="C221" s="9" t="s">
-        <v>339</v>
+      <c r="C221" s="2" t="s">
+        <v>332</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E221" s="38" t="s">
         <v>283</v>
       </c>
       <c r="F221" s="5"/>
     </row>
-    <row r="222" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="15"/>
-      <c r="B222" s="24"/>
-      <c r="C222" s="7" t="s">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="13"/>
+      <c r="B222" s="23"/>
+      <c r="C222" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D222" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E222" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="F222" s="5"/>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" s="13"/>
+      <c r="B223" s="23"/>
+      <c r="C223" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D223" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="E223" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="F223" s="5"/>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="13"/>
+      <c r="B224" s="23"/>
+      <c r="C224" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D224" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="E224" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="F224" s="5"/>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="13"/>
+      <c r="B225" s="23"/>
+      <c r="C225" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E225" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="F225" s="5"/>
+    </row>
+    <row r="226" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="15"/>
+      <c r="B226" s="24"/>
+      <c r="C226" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="D222" s="7" t="s">
+      <c r="D226" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="E222" s="51" t="s">
+      <c r="E226" s="51" t="s">
         <v>283</v>
       </c>
-      <c r="F222" s="8"/>
+      <c r="F226" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Meta not letting me pull
</commit_message>
<xml_diff>
--- a/Documentation/Asset list & planning.xlsx
+++ b/Documentation/Asset list & planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="400">
   <si>
     <t>Probation Area</t>
   </si>
@@ -1171,9 +1171,6 @@
   </si>
   <si>
     <t>3D_ENV_CLASS_Surveypaper</t>
-  </si>
-  <si>
-    <t>3D_EN_STOR_Ladder</t>
   </si>
   <si>
     <t>3D_ENV_GEN_RoomSigns</t>
@@ -1908,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E209" sqref="E209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,8 +2104,8 @@
       <c r="E7" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="F7" s="38" t="s">
-        <v>283</v>
+      <c r="F7" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="2"/>
@@ -2209,8 +2206,8 @@
       <c r="E10" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F10" s="38" t="s">
-        <v>283</v>
+      <c r="F10" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="2"/>
@@ -3015,8 +3012,8 @@
       <c r="E36" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="F36" s="38" t="s">
-        <v>283</v>
+      <c r="F36" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="2"/>
@@ -3045,8 +3042,8 @@
       <c r="E37" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="F37" s="38" t="s">
-        <v>283</v>
+      <c r="F37" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="2"/>
@@ -3195,8 +3192,8 @@
       <c r="E42" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="F42" s="38" t="s">
-        <v>283</v>
+      <c r="F42" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="G42" s="8"/>
       <c r="H42" s="2"/>
@@ -3249,8 +3246,8 @@
       <c r="E44" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F44" s="38" t="s">
-        <v>283</v>
+      <c r="F44" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="G44" s="5"/>
       <c r="H44" s="2"/>
@@ -3341,8 +3338,8 @@
       <c r="E47" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="F47" s="38" t="s">
-        <v>283</v>
+      <c r="F47" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>165</v>
@@ -4334,10 +4331,10 @@
       <c r="A87" s="14"/>
       <c r="B87" s="1"/>
       <c r="C87" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E87" s="9" t="s">
         <v>232</v>
@@ -4349,10 +4346,10 @@
       <c r="A88" s="14"/>
       <c r="B88" s="1"/>
       <c r="C88" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>232</v>
@@ -4364,10 +4361,10 @@
       <c r="A89" s="14"/>
       <c r="B89" s="1"/>
       <c r="C89" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>232</v>
@@ -4379,10 +4376,10 @@
       <c r="A90" s="14"/>
       <c r="B90" s="1"/>
       <c r="C90" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>232</v>
@@ -4394,10 +4391,10 @@
       <c r="A91" s="14"/>
       <c r="B91" s="1"/>
       <c r="C91" s="9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E91" s="9" t="s">
         <v>232</v>
@@ -4409,10 +4406,10 @@
       <c r="A92" s="14"/>
       <c r="B92" s="1"/>
       <c r="C92" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>232</v>
@@ -4424,10 +4421,10 @@
       <c r="A93" s="14"/>
       <c r="B93" s="1"/>
       <c r="C93" s="9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E93" s="9" t="s">
         <v>232</v>
@@ -4439,10 +4436,10 @@
       <c r="A94" s="14"/>
       <c r="B94" s="6"/>
       <c r="C94" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E94" s="9" t="s">
         <v>232</v>
@@ -5947,8 +5944,8 @@
       <c r="D204" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="E204" s="38" t="s">
-        <v>283</v>
+      <c r="E204" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="F204" s="5"/>
     </row>
@@ -5961,8 +5958,8 @@
       <c r="D205" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="E205" s="38" t="s">
-        <v>283</v>
+      <c r="E205" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="F205" s="5"/>
     </row>
@@ -5975,8 +5972,8 @@
       <c r="D206" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="E206" s="38" t="s">
-        <v>283</v>
+      <c r="E206" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="F206" s="5"/>
     </row>
@@ -6017,8 +6014,8 @@
       <c r="D209" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E209" s="38" t="s">
-        <v>283</v>
+      <c r="E209" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="F209" s="5"/>
     </row>
@@ -6173,8 +6170,8 @@
       <c r="D221" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E221" s="38" t="s">
-        <v>283</v>
+      <c r="E221" s="37" t="s">
+        <v>282</v>
       </c>
       <c r="F221" s="5"/>
     </row>
@@ -6259,7 +6256,7 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6516,7 +6513,7 @@
         <v>324</v>
       </c>
       <c r="F11" s="45" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G11" s="41"/>
       <c r="H11" s="45"/>
@@ -6764,9 +6761,11 @@
         <v>117</v>
       </c>
       <c r="F23" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="G23" s="41"/>
+        <v>142</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>116</v>
+      </c>
       <c r="H23" s="45"/>
       <c r="I23" s="41"/>
       <c r="J23" s="45"/>
@@ -6790,7 +6789,9 @@
       <c r="F24" s="45" t="s">
         <v>381</v>
       </c>
-      <c r="G24" s="41"/>
+      <c r="G24" s="41" t="s">
+        <v>183</v>
+      </c>
       <c r="H24" s="45"/>
       <c r="I24" s="41"/>
       <c r="J24" s="45"/>
@@ -6830,12 +6831,8 @@
         <v>145</v>
       </c>
       <c r="D26" s="45"/>
-      <c r="E26" s="41" t="s">
-        <v>382</v>
-      </c>
-      <c r="F26" s="45" t="s">
-        <v>116</v>
-      </c>
+      <c r="E26" s="41"/>
+      <c r="F26" s="45"/>
       <c r="G26" s="41"/>
       <c r="H26" s="45"/>
       <c r="I26" s="41"/>
@@ -7082,7 +7079,7 @@
         <v>105</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E40" s="39" t="s">
         <v>160</v>

</xml_diff>

<commit_message>
planning + merge (?)
</commit_message>
<xml_diff>
--- a/Documentation/Asset list & planning.xlsx
+++ b/Documentation/Asset list & planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="399">
   <si>
     <t>Probation Area</t>
   </si>
@@ -1162,9 +1162,6 @@
   </si>
   <si>
     <t>Bookcase</t>
-  </si>
-  <si>
-    <t>3D_CHAR_Assistent1</t>
   </si>
   <si>
     <t>3D_ENV_GEN_TrashCan</t>
@@ -1905,7 +1902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E209" sqref="E209"/>
     </sheetView>
   </sheetViews>
@@ -4331,10 +4328,10 @@
       <c r="A87" s="14"/>
       <c r="B87" s="1"/>
       <c r="C87" s="9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E87" s="9" t="s">
         <v>232</v>
@@ -4346,10 +4343,10 @@
       <c r="A88" s="14"/>
       <c r="B88" s="1"/>
       <c r="C88" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>232</v>
@@ -4361,10 +4358,10 @@
       <c r="A89" s="14"/>
       <c r="B89" s="1"/>
       <c r="C89" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>232</v>
@@ -4376,10 +4373,10 @@
       <c r="A90" s="14"/>
       <c r="B90" s="1"/>
       <c r="C90" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>232</v>
@@ -4391,10 +4388,10 @@
       <c r="A91" s="14"/>
       <c r="B91" s="1"/>
       <c r="C91" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E91" s="9" t="s">
         <v>232</v>
@@ -4406,10 +4403,10 @@
       <c r="A92" s="14"/>
       <c r="B92" s="1"/>
       <c r="C92" s="9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>232</v>
@@ -4421,10 +4418,10 @@
       <c r="A93" s="14"/>
       <c r="B93" s="1"/>
       <c r="C93" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E93" s="9" t="s">
         <v>232</v>
@@ -4436,10 +4433,10 @@
       <c r="A94" s="14"/>
       <c r="B94" s="6"/>
       <c r="C94" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E94" s="9" t="s">
         <v>232</v>
@@ -6255,8 +6252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6513,7 +6510,7 @@
         <v>324</v>
       </c>
       <c r="F11" s="45" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G11" s="41"/>
       <c r="H11" s="45"/>
@@ -6787,7 +6784,7 @@
         <v>153</v>
       </c>
       <c r="F24" s="45" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G24" s="41" t="s">
         <v>183</v>
@@ -6928,7 +6925,7 @@
         <v>52</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D32" s="45"/>
       <c r="E32" s="49"/>
@@ -7011,10 +7008,10 @@
         <v>231</v>
       </c>
       <c r="F36" s="44" t="s">
-        <v>223</v>
-      </c>
-      <c r="G36" s="47" t="s">
-        <v>379</v>
+        <v>315</v>
+      </c>
+      <c r="G36" s="39" t="s">
+        <v>315</v>
       </c>
       <c r="H36" s="48"/>
       <c r="I36" s="39"/>
@@ -7079,7 +7076,7 @@
         <v>105</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E40" s="39" t="s">
         <v>160</v>
@@ -7087,8 +7084,12 @@
       <c r="F40" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="G40" s="39"/>
-      <c r="H40" s="44"/>
+      <c r="G40" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="H40" s="48" t="s">
+        <v>182</v>
+      </c>
       <c r="I40" s="39"/>
       <c r="J40" s="44"/>
       <c r="K40" s="39"/>
@@ -7107,8 +7108,12 @@
       <c r="F41" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="G41" s="41"/>
-      <c r="H41" s="45"/>
+      <c r="G41" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="H41" s="45" t="s">
+        <v>158</v>
+      </c>
       <c r="I41" s="41"/>
       <c r="J41" s="45"/>
       <c r="K41" s="41"/>
@@ -7125,8 +7130,12 @@
       <c r="F42" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="G42" s="41"/>
-      <c r="H42" s="45"/>
+      <c r="G42" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="H42" s="45" t="s">
+        <v>159</v>
+      </c>
       <c r="I42" s="41"/>
       <c r="J42" s="45"/>
       <c r="K42" s="41"/>

</xml_diff>